<commit_message>
all experiments are run with main vector as reference point
</commit_message>
<xml_diff>
--- a/results/RMV/results.xlsx
+++ b/results/RMV/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-riaktu\IdeaProjects\graph2vec\results\RMV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54193B85-F0BB-4CD4-BCCA-0A9E8BC91370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F06EFE4-ABE1-43CA-A305-A289535C6AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -512,7 +512,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -1363,6 +1364,395 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>dists!$D$2:$D$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>7.2636382451270203</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.20294344494814</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.4626047367582</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.0526731864922603</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.5495322192039902</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.9569135808254101</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0483139745315</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.2201856823979202</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.9499309974567103</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.1543008109343003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.0550024453251794</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12.1367944223345</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.7769866306463395</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14.6438946363933</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.7520308369676698</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.6613510297540599</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.5026685346843403</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.6067888397129302</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.18276397986532</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.4675725012665701</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.5643966339706097</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.6390280558633599</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.8208475749158302</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.9828769700643996</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.3585981985413804</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7.9542264902266497</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.7970065255019296</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.5847436832082797</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6.0743140956013697</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6.77646056421362</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7.2041700257210204</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7.4521585639709196</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>7.0345519925807301</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6.92708076614469</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7.39326478325704</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6.8173149899101997</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7.1383241726462101</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8.00272404641583</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>7.0128200424498903</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.5664776522881301</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>7.5087595707538801</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7.1645963493380496</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>7.0411634335843196</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>6.3506972783011104</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.21034536087791</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>6.4542045327026596</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.43076871535545</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>8.6960995966534504</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2B49-4341-8F5E-659161CDE5BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="548557904"/>
+        <c:axId val="548534192"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="548557904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="548534192"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="548534192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="548557904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1443,6 +1833,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1960,6 +2390,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2546,6 +3492,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FACDD21-3F85-4B0C-A3FC-B753649129D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2854,7 +3838,7 @@
   <dimension ref="A1:AE51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2878,6 +3862,9 @@
       <c r="C2" s="1">
         <v>2.62489994863979E-3</v>
       </c>
+      <c r="D2" s="2">
+        <v>7.2636382451270203</v>
+      </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
@@ -2889,6 +3876,9 @@
       <c r="C3" s="1">
         <v>3.4140970031925001E-3</v>
       </c>
+      <c r="D3" s="2">
+        <v>7.20294344494814</v>
+      </c>
       <c r="AE3" t="s">
         <v>0</v>
       </c>
@@ -2903,6 +3893,9 @@
       <c r="C4" s="1">
         <v>2.46909841959708E-3</v>
       </c>
+      <c r="D4" s="2">
+        <v>7.4626047367582</v>
+      </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
@@ -2914,6 +3907,9 @@
       <c r="C5" s="1">
         <v>4.5037004525045801E-3</v>
       </c>
+      <c r="D5" s="2">
+        <v>7.0526731864922603</v>
+      </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
@@ -2925,6 +3921,9 @@
       <c r="C6" s="1">
         <v>4.7427463390257697E-2</v>
       </c>
+      <c r="D6" s="2">
+        <v>6.5495322192039902</v>
+      </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
@@ -2936,6 +3935,9 @@
       <c r="C7" s="1">
         <v>0.18064721685792101</v>
       </c>
+      <c r="D7" s="2">
+        <v>4.9569135808254101</v>
+      </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
@@ -2947,6 +3949,7 @@
       <c r="C8" s="1">
         <v>0.176988173698957</v>
       </c>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
@@ -2958,6 +3961,9 @@
       <c r="C9" s="1">
         <v>0.25399654972261698</v>
       </c>
+      <c r="D9" s="2">
+        <v>1.0483139745315</v>
+      </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
@@ -2969,6 +3975,9 @@
       <c r="C10" s="1">
         <v>0.241731148871459</v>
       </c>
+      <c r="D10" s="2">
+        <v>8.2201856823979202</v>
+      </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
@@ -2980,6 +3989,9 @@
       <c r="C11" s="1">
         <v>0.22399775835101299</v>
       </c>
+      <c r="D11" s="2">
+        <v>7.9499309974567103</v>
+      </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
@@ -2991,6 +4003,9 @@
       <c r="C12" s="1">
         <v>0.21479485925723199</v>
       </c>
+      <c r="D12" s="2">
+        <v>5.1543008109343003</v>
+      </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
@@ -3002,6 +4017,7 @@
       <c r="C13" s="1">
         <v>0.29140043760337803</v>
       </c>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
@@ -3013,6 +4029,9 @@
       <c r="C14" s="1">
         <v>0.285874893110038</v>
       </c>
+      <c r="D14" s="2">
+        <v>8.0550024453251794</v>
+      </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
@@ -3024,6 +4043,9 @@
       <c r="C15" s="1">
         <v>0.23812259509209499</v>
       </c>
+      <c r="D15" s="2">
+        <v>12.1367944223345</v>
+      </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
@@ -3035,8 +4057,11 @@
       <c r="C16" s="1">
         <v>0.17906098483261701</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D16" s="2">
+        <v>8.7769866306463395</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -3046,8 +4071,11 @@
       <c r="C17" s="1">
         <v>0.246024379847647</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D17" s="2">
+        <v>14.6438946363933</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -3057,8 +4085,11 @@
       <c r="C18" s="1">
         <v>0.19443424585098601</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D18" s="2">
+        <v>9.7520308369676698</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -3068,8 +4099,11 @@
       <c r="C19" s="1">
         <v>0.116282699106666</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D19" s="2">
+        <v>3.6613510297540599</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -3079,8 +4113,11 @@
       <c r="C20" s="1">
         <v>0.18453189088028599</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D20" s="2">
+        <v>6.5026685346843403</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -3090,8 +4127,11 @@
       <c r="C21" s="1">
         <v>0.23970781938164101</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D21" s="2">
+        <v>3.6067888397129302</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -3101,8 +4141,11 @@
       <c r="C22" s="1">
         <v>0.14148419412163599</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D22" s="2">
+        <v>4.18276397986532</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -3112,8 +4155,11 @@
       <c r="C23" s="1">
         <v>0.24522768891434199</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D23" s="2">
+        <v>4.4675725012665701</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -3123,8 +4169,11 @@
       <c r="C24" s="1">
         <v>9.2828034029826895E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D24" s="2">
+        <v>9.5643966339706097</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -3134,8 +4183,11 @@
       <c r="C25" s="1">
         <v>0.112360130710315</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D25" s="2">
+        <v>5.6390280558633599</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -3145,8 +4197,11 @@
       <c r="C26" s="1">
         <v>9.6912540119162893E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D26" s="2">
+        <v>5.8208475749158302</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -3156,8 +4211,11 @@
       <c r="C27" s="1">
         <v>4.40407258014811E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D27" s="2">
+        <v>6.9828769700643996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -3167,8 +4225,11 @@
       <c r="C28" s="1">
         <v>2.6314785409043501E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D28" s="2">
+        <v>7.3585981985413804</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -3178,8 +4239,11 @@
       <c r="C29" s="1">
         <v>9.3080750184183894E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D29" s="2">
+        <v>7.9542264902266497</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -3189,8 +4253,11 @@
       <c r="C30" s="1">
         <v>4.8333642098000701E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D30" s="2">
+        <v>7.7970065255019296</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -3200,8 +4267,11 @@
       <c r="C31" s="1">
         <v>4.9538252647470998E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D31" s="2">
+        <v>5.5847436832082797</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -3211,8 +4281,11 @@
       <c r="C32" s="1">
         <v>3.2945074016049403E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D32" s="2">
+        <v>6.0743140956013697</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -3222,8 +4295,11 @@
       <c r="C33" s="1">
         <v>3.3603386629144902E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D33" s="2">
+        <v>6.77646056421362</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -3233,8 +4309,11 @@
       <c r="C34" s="1">
         <v>1.651529153441E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D34" s="2">
+        <v>7.2041700257210204</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -3244,8 +4323,11 @@
       <c r="C35" s="1">
         <v>3.5936052447446298E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D35" s="2">
+        <v>7.4521585639709196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -3255,8 +4337,11 @@
       <c r="C36" s="1">
         <v>2.1792203657770199E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D36" s="2">
+        <v>7.0345519925807301</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -3266,8 +4351,11 @@
       <c r="C37" s="1">
         <v>2.4064210381691101E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D37" s="2">
+        <v>6.92708076614469</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -3277,8 +4365,11 @@
       <c r="C38" s="1">
         <v>2.4161679442739802E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D38" s="2">
+        <v>7.39326478325704</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -3288,8 +4379,11 @@
       <c r="C39" s="1">
         <v>1.9910364511976E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D39" s="2">
+        <v>6.8173149899101997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -3299,8 +4393,11 @@
       <c r="C40" s="1">
         <v>9.0597252643395097E-3</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D40" s="2">
+        <v>7.1383241726462101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3310,8 +4407,11 @@
       <c r="C41" s="1">
         <v>8.0949428900704001E-3</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D41" s="2">
+        <v>8.00272404641583</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3321,8 +4421,11 @@
       <c r="C42" s="1">
         <v>1.0591952023571501E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D42" s="2">
+        <v>7.0128200424498903</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -3332,8 +4435,11 @@
       <c r="C43" s="1">
         <v>1.7448592207499499E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D43" s="2">
+        <v>5.5664776522881301</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -3343,8 +4449,11 @@
       <c r="C44" s="1">
         <v>9.1866280760892708E-3</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D44" s="2">
+        <v>7.5087595707538801</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -3354,8 +4463,11 @@
       <c r="C45" s="1">
         <v>9.9559702516720493E-3</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D45" s="2">
+        <v>7.1645963493380496</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -3365,8 +4477,11 @@
       <c r="C46" s="1">
         <v>6.5584907002026399E-3</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D46" s="2">
+        <v>7.0411634335843196</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -3376,8 +4491,11 @@
       <c r="C47" s="1">
         <v>3.5187406718788501E-3</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D47" s="2">
+        <v>6.3506972783011104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -3387,8 +4505,11 @@
       <c r="C48" s="1">
         <v>4.1417905211466001E-3</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D48" s="2">
+        <v>4.21034536087791</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -3398,8 +4519,11 @@
       <c r="C49" s="1">
         <v>4.2854481393716998E-3</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D49" s="2">
+        <v>6.4542045327026596</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -3409,8 +4533,11 @@
       <c r="C50" s="1">
         <v>3.1903688322001398E-3</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D50" s="2">
+        <v>2.43076871535545</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -3419,6 +4546,9 @@
       </c>
       <c r="C51" s="1">
         <v>0.46333263449570999</v>
+      </c>
+      <c r="D51" s="2">
+        <v>8.6960995966534504</v>
       </c>
     </row>
   </sheetData>

</xml_diff>